<commit_message>
add comments to update ilog
</commit_message>
<xml_diff>
--- a/input/binomial-crosswalk.xlsx
+++ b/input/binomial-crosswalk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\wildlife-cameras\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E96044-ECC3-4BF5-9809-E52E1C52A248}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC9A0FD-B63D-4BD7-B944-035C22A9E5F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="2475" windowWidth="20085" windowHeight="7050" tabRatio="648" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2220" yWindow="2475" windowWidth="20085" windowHeight="7050" tabRatio="648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="photo-type_binomial_DEN" sheetId="12" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'error-dictionary'!$A$1:$C$21</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">legacy!$A$1:$H$624</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'legacy_2023-11-01'!$A$1:$I$798</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'photo-type_binomial'!$A$1:$J$1033</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'photo-type_binomial'!$A$1:$J$1034</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'photo-type_binomial_DEN'!$A$1:$J$124</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -14035,9 +14035,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J1034"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1035" sqref="I1035"/>
+      <selection pane="bottomLeft" activeCell="A1035" sqref="A1035:XFD1035"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -18756,7 +18756,7 @@
       </c>
       <c r="J178" s="27"/>
     </row>
-    <row r="179" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="27" t="s">
         <v>2</v>
       </c>
@@ -35096,7 +35096,7 @@
       <c r="I739" s="47"/>
       <c r="J739" s="27"/>
     </row>
-    <row r="740" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="740" spans="1:10" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A740" s="27" t="s">
         <v>50</v>
       </c>
@@ -43928,7 +43928,7 @@
       </c>
       <c r="J1033" s="27"/>
     </row>
-    <row r="1034" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1034" spans="1:10" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1034" s="27" t="s">
         <v>50</v>
       </c>
@@ -43957,10 +43957,10 @@
       <c r="J1034" s="27"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1033" xr:uid="{11F9BBD1-A794-482F-8733-C6568E26B364}">
-    <filterColumn colId="0">
+  <autoFilter ref="A1:J1034" xr:uid="{11F9BBD1-A794-482F-8733-C6568E26B364}">
+    <filterColumn colId="2">
       <filters>
-        <filter val="Needs ID"/>
+        <filter val="Animal_Rodent species"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -44084,20 +44084,20 @@
     <cfRule type="duplicateValues" dxfId="49" priority="1852"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1034">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1034">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1034">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1034">
-    <cfRule type="duplicateValues" dxfId="1" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1034">
-    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="6"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -44369,7 +44369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFDC6CD0-BBAC-F848-A64B-A20370559F7C}">
   <dimension ref="A1:E201"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
     </sheetView>
@@ -47058,89 +47058,89 @@
     <sortCondition ref="B2:B201"/>
   </sortState>
   <conditionalFormatting sqref="A202:A1048576 A91:A106 A1:A84">
-    <cfRule type="duplicateValues" dxfId="48" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A202:A1048576 A1:A106">
-    <cfRule type="duplicateValues" dxfId="47" priority="50"/>
-    <cfRule type="duplicateValues" dxfId="46" priority="51"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="50"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="51"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A202:A1048576 A1:A106">
-    <cfRule type="duplicateValues" dxfId="45" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A202:A1048576 A1:A119">
-    <cfRule type="duplicateValues" dxfId="44" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A193 A202:A1048576">
-    <cfRule type="duplicateValues" dxfId="43" priority="24"/>
-    <cfRule type="duplicateValues" dxfId="42" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A107">
-    <cfRule type="duplicateValues" dxfId="41" priority="1246"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="1246"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A107">
-    <cfRule type="duplicateValues" dxfId="40" priority="1247"/>
-    <cfRule type="duplicateValues" dxfId="39" priority="1248"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="1247"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="1248"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A108:A119">
-    <cfRule type="duplicateValues" dxfId="38" priority="1441"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="1441"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C149:C159">
-    <cfRule type="duplicateValues" dxfId="37" priority="1457"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="1457"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A149:A193 A124:A141">
-    <cfRule type="duplicateValues" dxfId="36" priority="1668"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="1668"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A124:A193">
-    <cfRule type="duplicateValues" dxfId="35" priority="1671"/>
-    <cfRule type="duplicateValues" dxfId="34" priority="1672"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="1671"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="1672"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A120:A193">
-    <cfRule type="duplicateValues" dxfId="33" priority="1675"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="1675"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A194">
-    <cfRule type="duplicateValues" dxfId="32" priority="18"/>
-    <cfRule type="duplicateValues" dxfId="31" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A194">
-    <cfRule type="duplicateValues" dxfId="30" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A194">
-    <cfRule type="duplicateValues" dxfId="29" priority="21"/>
-    <cfRule type="duplicateValues" dxfId="28" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A194">
-    <cfRule type="duplicateValues" dxfId="27" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A195">
-    <cfRule type="duplicateValues" dxfId="26" priority="12"/>
-    <cfRule type="duplicateValues" dxfId="25" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A195">
-    <cfRule type="duplicateValues" dxfId="24" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A195">
-    <cfRule type="duplicateValues" dxfId="23" priority="15"/>
-    <cfRule type="duplicateValues" dxfId="22" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A195">
-    <cfRule type="duplicateValues" dxfId="21" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A196">
-    <cfRule type="duplicateValues" dxfId="20" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="19" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A196">
-    <cfRule type="duplicateValues" dxfId="18" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A196">
-    <cfRule type="duplicateValues" dxfId="17" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="16" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A196">
-    <cfRule type="duplicateValues" dxfId="15" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="14" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -84938,16 +84938,16 @@
     <sortCondition ref="E2:E621"/>
   </sortState>
   <conditionalFormatting sqref="C1:C621 C625:C1048576">
-    <cfRule type="duplicateValues" dxfId="13" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C622:C623">
-    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C624">
-    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -85326,10 +85326,10 @@
   </sheetData>
   <autoFilter ref="B1:C31" xr:uid="{FB598717-82D7-48E5-A54E-FB6A5DEF5ACB}"/>
   <conditionalFormatting sqref="C30">
-    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -86674,10 +86674,10 @@
     <sortCondition ref="D2:D75"/>
   </sortState>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>